<commit_message>
Add header row to assignments
</commit_message>
<xml_diff>
--- a/src/ACAT/assignments/FA24/COMP-101_FA24_01_assignments.xlsx
+++ b/src/ACAT/assignments/FA24/COMP-101_FA24_01_assignments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jglossner\GitRivier\Assessment\src\ACAT\assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jglossner\GitRivier\Assessment\src\ACAT\assignments\FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1E48135-3F1A-4561-8DFF-5FB0231D3987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3155480-280E-470D-B0EF-6D97A0A0E591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="1995" windowWidth="21600" windowHeight="11025" xr2:uid="{B92A6C1B-03A8-46E2-9EF8-B66F995B4D20}"/>
+    <workbookView xWindow="2880" yWindow="1650" windowWidth="21600" windowHeight="11025" xr2:uid="{B92A6C1B-03A8-46E2-9EF8-B66F995B4D20}"/>
   </bookViews>
   <sheets>
     <sheet name="COMP-101" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Demonstrate understanding of primitive data types, control structures, and simple input-output operations.</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Test and debug programs to ensure correctness and efficiency.</t>
+  </si>
+  <si>
+    <t>Course Outcome</t>
+  </si>
+  <si>
+    <t>Assignment 1</t>
+  </si>
+  <si>
+    <t>Assignment 2</t>
   </si>
 </sst>
 </file>
@@ -455,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F4D45A-8940-44D9-BA4F-E755B26CB856}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -468,20 +477,20 @@
     <col min="3" max="16384" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -492,7 +501,7 @@
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -503,7 +512,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -512,8 +521,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -526,6 +543,9 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Update column names to match Canvas
</commit_message>
<xml_diff>
--- a/src/ACAT/assignments/FA24/COMP-101_FA24_01_assignments.xlsx
+++ b/src/ACAT/assignments/FA24/COMP-101_FA24_01_assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jglossner\GitRivier\Assessment\src\ACAT\assignments\FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3155480-280E-470D-B0EF-6D97A0A0E591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397B3C7B-7D27-4E5D-B659-C2DCD13D6431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1650" windowWidth="21600" windowHeight="11025" xr2:uid="{B92A6C1B-03A8-46E2-9EF8-B66F995B4D20}"/>
+    <workbookView xWindow="525" yWindow="4335" windowWidth="21600" windowHeight="11025" xr2:uid="{B92A6C1B-03A8-46E2-9EF8-B66F995B4D20}"/>
   </bookViews>
   <sheets>
     <sheet name="COMP-101" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>Demonstrate understanding of primitive data types, control structures, and simple input-output operations.</t>
   </si>
   <si>
-    <t>Final Exam</t>
-  </si>
-  <si>
-    <t>Final Project</t>
-  </si>
-  <si>
     <t>Apply problem-solving and algorithmic solutions to create functional programs.</t>
   </si>
   <si>
@@ -63,6 +57,12 @@
   </si>
   <si>
     <t>Assignment 2</t>
+  </si>
+  <si>
+    <t>Exams Final Score</t>
+  </si>
+  <si>
+    <t>Projects Final Score</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -479,13 +479,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -493,43 +493,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>